<commit_message>
[Angular][ShippingMS] Update Import Shipping Plan - Work Order  - Layout
</commit_message>
<xml_diff>
--- a/Microservices/FilesMicroservice/Files.Api/wwwroot/test/WorkOrderTemplate-test-2.xlsx
+++ b/Microservices/FilesMicroservice/Files.Api/wwwroot/test/WorkOrderTemplate-test-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Khoa\Desktop\spatronics-shipping-application\Microservices\FilesMicroservice\Files.Api\wwwroot\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B0F25B4-BF8B-426C-906C-1D07577C02DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF35BDF-5B51-400E-8140-C6CE6D49F873}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="89">
   <si>
     <t>WorkOrderId</t>
   </si>
@@ -37,654 +37,153 @@
     <t>ABCD232332</t>
   </si>
   <si>
-    <t>ABC2394984932</t>
-  </si>
-  <si>
-    <t>ABCD232333</t>
-  </si>
-  <si>
-    <t>ABC2394984933</t>
-  </si>
-  <si>
-    <t>ABCD232334</t>
-  </si>
-  <si>
-    <t>ABC2394984934</t>
-  </si>
-  <si>
-    <t>ABCD232335</t>
-  </si>
-  <si>
-    <t>ABC2394984935</t>
-  </si>
-  <si>
-    <t>ABCD232336</t>
-  </si>
-  <si>
-    <t>ABC2394984936</t>
-  </si>
-  <si>
-    <t>ABCD232337</t>
-  </si>
-  <si>
-    <t>ABC2394984937</t>
-  </si>
-  <si>
-    <t>ABCD232338</t>
-  </si>
-  <si>
-    <t>ABC2394984938</t>
-  </si>
-  <si>
-    <t>ABCD232339</t>
-  </si>
-  <si>
-    <t>ABC2394984939</t>
-  </si>
-  <si>
     <t>ABCD232340</t>
   </si>
   <si>
-    <t>ABC2394984940</t>
-  </si>
-  <si>
-    <t>ABCD232341</t>
-  </si>
-  <si>
-    <t>ABC2394984941</t>
-  </si>
-  <si>
-    <t>ABCD232342</t>
-  </si>
-  <si>
-    <t>ABC2394984942</t>
-  </si>
-  <si>
-    <t>ABCD232343</t>
-  </si>
-  <si>
-    <t>ABC2394984943</t>
-  </si>
-  <si>
-    <t>ABCD232344</t>
-  </si>
-  <si>
-    <t>ABC2394984944</t>
-  </si>
-  <si>
-    <t>ABCD232345</t>
-  </si>
-  <si>
-    <t>ABC2394984945</t>
-  </si>
-  <si>
-    <t>ABCD232346</t>
-  </si>
-  <si>
-    <t>ABC2394984946</t>
-  </si>
-  <si>
-    <t>ABCD232347</t>
-  </si>
-  <si>
-    <t>ABC2394984947</t>
-  </si>
-  <si>
-    <t>ABCD232348</t>
-  </si>
-  <si>
-    <t>ABC2394984948</t>
-  </si>
-  <si>
-    <t>ABCD232349</t>
-  </si>
-  <si>
-    <t>ABC2394984949</t>
-  </si>
-  <si>
     <t>ABCD232350</t>
   </si>
   <si>
-    <t>ABC2394984950</t>
-  </si>
-  <si>
-    <t>ABCD232351</t>
-  </si>
-  <si>
-    <t>ABC2394984951</t>
-  </si>
-  <si>
-    <t>ABCD232352</t>
-  </si>
-  <si>
-    <t>ABC2394984952</t>
-  </si>
-  <si>
-    <t>ABCD232353</t>
-  </si>
-  <si>
-    <t>ABC2394984953</t>
-  </si>
-  <si>
-    <t>ABCD232354</t>
-  </si>
-  <si>
-    <t>ABC2394984954</t>
-  </si>
-  <si>
-    <t>ABCD232355</t>
-  </si>
-  <si>
-    <t>ABC2394984955</t>
-  </si>
-  <si>
-    <t>ABCD232356</t>
-  </si>
-  <si>
-    <t>ABC2394984956</t>
-  </si>
-  <si>
-    <t>ABCD232357</t>
-  </si>
-  <si>
-    <t>ABC2394984957</t>
-  </si>
-  <si>
-    <t>ABCD232358</t>
-  </si>
-  <si>
-    <t>ABC2394984958</t>
-  </si>
-  <si>
-    <t>ABCD232359</t>
-  </si>
-  <si>
-    <t>ABC2394984959</t>
-  </si>
-  <si>
     <t>ABCD232360</t>
   </si>
   <si>
-    <t>ABC2394984960</t>
-  </si>
-  <si>
-    <t>ABCD232361</t>
-  </si>
-  <si>
-    <t>ABC2394984961</t>
-  </si>
-  <si>
-    <t>ABCD232362</t>
-  </si>
-  <si>
-    <t>ABC2394984962</t>
-  </si>
-  <si>
-    <t>ABCD232363</t>
-  </si>
-  <si>
-    <t>ABC2394984963</t>
-  </si>
-  <si>
-    <t>ABCD232364</t>
-  </si>
-  <si>
-    <t>ABC2394984964</t>
-  </si>
-  <si>
-    <t>ABCD232365</t>
-  </si>
-  <si>
-    <t>ABC2394984965</t>
-  </si>
-  <si>
-    <t>ABCD232366</t>
-  </si>
-  <si>
-    <t>ABC2394984966</t>
-  </si>
-  <si>
-    <t>ABCD232367</t>
-  </si>
-  <si>
-    <t>ABC2394984967</t>
-  </si>
-  <si>
-    <t>ABCD232368</t>
-  </si>
-  <si>
-    <t>ABC2394984968</t>
-  </si>
-  <si>
-    <t>ABCD232369</t>
-  </si>
-  <si>
-    <t>ABC2394984969</t>
-  </si>
-  <si>
     <t>ABCD232370</t>
   </si>
   <si>
-    <t>ABC2394984970</t>
-  </si>
-  <si>
-    <t>ABCD232371</t>
-  </si>
-  <si>
-    <t>ABC2394984971</t>
-  </si>
-  <si>
-    <t>ABCD232372</t>
-  </si>
-  <si>
-    <t>ABC2394984972</t>
-  </si>
-  <si>
-    <t>ABCD232373</t>
-  </si>
-  <si>
-    <t>ABC2394984973</t>
-  </si>
-  <si>
-    <t>ABCD232374</t>
-  </si>
-  <si>
-    <t>ABC2394984974</t>
-  </si>
-  <si>
-    <t>ABCD232375</t>
-  </si>
-  <si>
-    <t>ABC2394984975</t>
-  </si>
-  <si>
-    <t>ABCD232376</t>
-  </si>
-  <si>
-    <t>ABC2394984976</t>
-  </si>
-  <si>
-    <t>ABCD232377</t>
-  </si>
-  <si>
-    <t>ABC2394984977</t>
-  </si>
-  <si>
     <t>ABCD232378</t>
   </si>
   <si>
-    <t>ABC2394984978</t>
-  </si>
-  <si>
-    <t>ABCD232379</t>
-  </si>
-  <si>
-    <t>ABC2394984979</t>
-  </si>
-  <si>
-    <t>ABCD232380</t>
-  </si>
-  <si>
-    <t>ABC2394984980</t>
-  </si>
-  <si>
-    <t>ABCD232381</t>
-  </si>
-  <si>
-    <t>ABC2394984981</t>
-  </si>
-  <si>
-    <t>ABCD232382</t>
-  </si>
-  <si>
-    <t>ABC2394984982</t>
-  </si>
-  <si>
-    <t>ABCD232383</t>
-  </si>
-  <si>
-    <t>ABC2394984983</t>
-  </si>
-  <si>
-    <t>ABCD232384</t>
-  </si>
-  <si>
-    <t>ABC2394984984</t>
-  </si>
-  <si>
-    <t>ABCD232385</t>
-  </si>
-  <si>
-    <t>ABC2394984985</t>
-  </si>
-  <si>
-    <t>ABCD232386</t>
-  </si>
-  <si>
-    <t>ABC2394984986</t>
-  </si>
-  <si>
-    <t>ABCD232387</t>
-  </si>
-  <si>
-    <t>ABC2394984987</t>
-  </si>
-  <si>
-    <t>ABCD232388</t>
-  </si>
-  <si>
-    <t>ABC2394984988</t>
-  </si>
-  <si>
     <t>ABCD232389</t>
   </si>
   <si>
-    <t>ABC2394984989</t>
-  </si>
-  <si>
-    <t>ABCD232390</t>
-  </si>
-  <si>
-    <t>ABC2394984990</t>
-  </si>
-  <si>
-    <t>ABCD232391</t>
-  </si>
-  <si>
-    <t>ABC2394984991</t>
-  </si>
-  <si>
-    <t>ABCD232392</t>
-  </si>
-  <si>
-    <t>ABC2394984992</t>
-  </si>
-  <si>
-    <t>ABCD232393</t>
-  </si>
-  <si>
-    <t>ABC2394984993</t>
-  </si>
-  <si>
-    <t>ABCD232394</t>
-  </si>
-  <si>
-    <t>ABC2394984994</t>
-  </si>
-  <si>
-    <t>ABCD232395</t>
-  </si>
-  <si>
-    <t>ABC2394984995</t>
-  </si>
-  <si>
-    <t>ABCD232396</t>
-  </si>
-  <si>
-    <t>ABC2394984996</t>
-  </si>
-  <si>
-    <t>ABCD232397</t>
-  </si>
-  <si>
     <t>ABC2394984997</t>
   </si>
   <si>
-    <t>ABCD232398</t>
-  </si>
-  <si>
     <t>ABC2394984998</t>
   </si>
   <si>
-    <t>ABCD232399</t>
-  </si>
-  <si>
     <t>ABC2394984999</t>
   </si>
   <si>
-    <t>ABCD232400</t>
-  </si>
-  <si>
     <t>ABC2394985000</t>
   </si>
   <si>
-    <t>ABCD232401</t>
-  </si>
-  <si>
     <t>ABC2394985001</t>
   </si>
   <si>
-    <t>ABCD232402</t>
-  </si>
-  <si>
     <t>ABC2394985002</t>
   </si>
   <si>
-    <t>ABCD232403</t>
-  </si>
-  <si>
     <t>ABC2394985003</t>
   </si>
   <si>
-    <t>ABCD232404</t>
-  </si>
-  <si>
     <t>ABC2394985004</t>
   </si>
   <si>
-    <t>ABCD232405</t>
-  </si>
-  <si>
     <t>ABC2394985005</t>
   </si>
   <si>
-    <t>ABCD232406</t>
-  </si>
-  <si>
     <t>ABC2394985006</t>
   </si>
   <si>
-    <t>ABCD232407</t>
-  </si>
-  <si>
     <t>ABC2394985007</t>
   </si>
   <si>
-    <t>ABCD232408</t>
-  </si>
-  <si>
     <t>ABC2394985008</t>
   </si>
   <si>
-    <t>ABCD232409</t>
-  </si>
-  <si>
     <t>ABC2394985009</t>
   </si>
   <si>
-    <t>ABCD232410</t>
-  </si>
-  <si>
     <t>ABC2394985010</t>
   </si>
   <si>
-    <t>ABCD232411</t>
-  </si>
-  <si>
     <t>ABC2394985011</t>
   </si>
   <si>
-    <t>ABCD232412</t>
-  </si>
-  <si>
     <t>ABC2394985012</t>
   </si>
   <si>
-    <t>ABCD232413</t>
-  </si>
-  <si>
     <t>ABC2394985013</t>
   </si>
   <si>
-    <t>ABCD232414</t>
-  </si>
-  <si>
     <t>ABC2394985014</t>
   </si>
   <si>
-    <t>ABCD232415</t>
-  </si>
-  <si>
     <t>ABC2394985015</t>
   </si>
   <si>
-    <t>ABCD232416</t>
-  </si>
-  <si>
     <t>ABC2394985016</t>
   </si>
   <si>
-    <t>ABCD232417</t>
-  </si>
-  <si>
     <t>ABC2394985017</t>
   </si>
   <si>
-    <t>ABCD232418</t>
-  </si>
-  <si>
     <t>ABC2394985018</t>
   </si>
   <si>
-    <t>ABCD232419</t>
-  </si>
-  <si>
     <t>ABC2394985019</t>
   </si>
   <si>
-    <t>ABCD232420</t>
-  </si>
-  <si>
     <t>ABC2394985020</t>
   </si>
   <si>
-    <t>ABCD232421</t>
-  </si>
-  <si>
     <t>ABC2394985021</t>
   </si>
   <si>
-    <t>ABCD232422</t>
-  </si>
-  <si>
     <t>ABC2394985022</t>
   </si>
   <si>
-    <t>ABCD232423</t>
-  </si>
-  <si>
     <t>ABC2394985023</t>
   </si>
   <si>
-    <t>ABCD232424</t>
-  </si>
-  <si>
     <t>ABC2394985024</t>
   </si>
   <si>
-    <t>ABCD232425</t>
-  </si>
-  <si>
     <t>ABC2394985025</t>
   </si>
   <si>
-    <t>ABCD232426</t>
-  </si>
-  <si>
     <t>ABC2394985026</t>
   </si>
   <si>
-    <t>ABCD232427</t>
-  </si>
-  <si>
     <t>ABC2394985027</t>
   </si>
   <si>
-    <t>ABCD232428</t>
-  </si>
-  <si>
     <t>ABC2394985028</t>
   </si>
   <si>
-    <t>ABCD232429</t>
-  </si>
-  <si>
     <t>ABC2394985029</t>
   </si>
   <si>
-    <t>ABCD232430</t>
-  </si>
-  <si>
     <t>ABC2394985030</t>
   </si>
   <si>
-    <t>ABCD232431</t>
-  </si>
-  <si>
     <t>ABC2394985031</t>
   </si>
   <si>
-    <t>ABCD232432</t>
-  </si>
-  <si>
     <t>ABC2394985032</t>
   </si>
   <si>
-    <t>ABCD232433</t>
-  </si>
-  <si>
     <t>ABC2394985033</t>
   </si>
   <si>
-    <t>ABCD232434</t>
-  </si>
-  <si>
     <t>ABC2394985034</t>
   </si>
   <si>
-    <t>ABCD232435</t>
-  </si>
-  <si>
     <t>ABC2394985035</t>
   </si>
   <si>
-    <t>ABCD232436</t>
-  </si>
-  <si>
     <t>ABC2394985036</t>
   </si>
   <si>
-    <t>ABCD232437</t>
-  </si>
-  <si>
     <t>ABC2394985037</t>
   </si>
   <si>
-    <t>ABCD232438</t>
-  </si>
-  <si>
     <t>ABC2394985038</t>
   </si>
   <si>
-    <t>ABCD232439</t>
-  </si>
-  <si>
     <t>ABC2394985039</t>
   </si>
   <si>
-    <t>ABCD232440</t>
-  </si>
-  <si>
     <t>ABC2394985040</t>
   </si>
   <si>
@@ -694,185 +193,107 @@
     <t>ABC2394985041</t>
   </si>
   <si>
-    <t>ABCD232442</t>
-  </si>
-  <si>
     <t>ABC2394985042</t>
   </si>
   <si>
-    <t>ABCD232443</t>
-  </si>
-  <si>
     <t>ABC2394985043</t>
   </si>
   <si>
-    <t>ABCD232444</t>
-  </si>
-  <si>
     <t>ABC2394985044</t>
   </si>
   <si>
-    <t>ABCD232445</t>
-  </si>
-  <si>
     <t>ABC2394985045</t>
   </si>
   <si>
-    <t>ABCD232446</t>
-  </si>
-  <si>
     <t>ABC2394985046</t>
   </si>
   <si>
-    <t>ABCD232447</t>
-  </si>
-  <si>
     <t>ABC2394985047</t>
   </si>
   <si>
-    <t>ABCD232448</t>
-  </si>
-  <si>
     <t>ABC2394985048</t>
   </si>
   <si>
-    <t>ABCD232449</t>
-  </si>
-  <si>
     <t>ABC2394985049</t>
   </si>
   <si>
-    <t>ABCD232450</t>
-  </si>
-  <si>
     <t>ABC2394985050</t>
   </si>
   <si>
-    <t>ABCD232451</t>
-  </si>
-  <si>
     <t>ABC2394985051</t>
   </si>
   <si>
-    <t>ABCD232452</t>
-  </si>
-  <si>
     <t>ABC2394985052</t>
   </si>
   <si>
-    <t>ABCD232453</t>
-  </si>
-  <si>
     <t>ABC2394985053</t>
   </si>
   <si>
-    <t>ABCD232454</t>
-  </si>
-  <si>
     <t>ABC2394985054</t>
   </si>
   <si>
-    <t>ABCD232455</t>
-  </si>
-  <si>
     <t>ABC2394985055</t>
   </si>
   <si>
-    <t>ABCD232456</t>
-  </si>
-  <si>
     <t>ABC2394985056</t>
   </si>
   <si>
-    <t>ABCD232457</t>
-  </si>
-  <si>
     <t>ABC2394985057</t>
   </si>
   <si>
-    <t>ABCD232458</t>
-  </si>
-  <si>
     <t>ABC2394985058</t>
   </si>
   <si>
-    <t>ABCD232459</t>
-  </si>
-  <si>
     <t>ABC2394985059</t>
   </si>
   <si>
-    <t>ABCD232460</t>
-  </si>
-  <si>
     <t>ABC2394985060</t>
   </si>
   <si>
-    <t>ABCD232461</t>
-  </si>
-  <si>
     <t>ABC2394985061</t>
   </si>
   <si>
-    <t>ABCD232462</t>
-  </si>
-  <si>
     <t>ABC2394985062</t>
   </si>
   <si>
-    <t>ABCD232463</t>
-  </si>
-  <si>
     <t>ABC2394985063</t>
   </si>
   <si>
-    <t>ABCD232464</t>
-  </si>
-  <si>
     <t>ABC2394985064</t>
   </si>
   <si>
-    <t>ABCD232465</t>
-  </si>
-  <si>
     <t>ABC2394985065</t>
   </si>
   <si>
-    <t>ABCD232466</t>
-  </si>
-  <si>
     <t>ABC2394985066</t>
   </si>
   <si>
-    <t>ABCD232467</t>
-  </si>
-  <si>
     <t>ABC2394985067</t>
   </si>
   <si>
-    <t>ABCD232468</t>
-  </si>
-  <si>
     <t>ABC2394985068</t>
   </si>
   <si>
-    <t>ABCD232469</t>
-  </si>
-  <si>
     <t>ABC2394985069</t>
   </si>
   <si>
-    <t>ABCD232470</t>
-  </si>
-  <si>
     <t>ABC2394985070</t>
+  </si>
+  <si>
+    <t>Product Number 3</t>
+  </si>
+  <si>
+    <t>Product Number 2</t>
+  </si>
+  <si>
+    <t>Product Number 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -880,6 +301,10 @@
     <font>
       <b/>
       <sz val="14"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -923,7 +348,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
@@ -938,6 +363,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1256,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A99" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1283,8 +711,8 @@
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>5</v>
+      <c r="B2" t="s">
+        <v>86</v>
       </c>
       <c r="C2" s="3">
         <v>2000</v>
@@ -1293,10 +721,10 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C3" s="3">
         <v>2000</v>
@@ -1305,10 +733,10 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C4" s="3">
         <v>2000</v>
@@ -1317,10 +745,10 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>11</v>
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C5" s="3">
         <v>2000</v>
@@ -1329,10 +757,10 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C6" s="3">
         <v>2000</v>
@@ -1341,10 +769,10 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C7" s="3">
         <v>2000</v>
@@ -1353,10 +781,10 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>17</v>
+        <v>4</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C8" s="3">
         <v>2000</v>
@@ -1365,10 +793,10 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>4</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C9" s="3">
         <v>2000</v>
@@ -1377,10 +805,10 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C10" s="3">
         <v>2000</v>
@@ -1389,10 +817,10 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C11" s="3">
         <v>2000</v>
@@ -1401,10 +829,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C12" s="3">
         <v>2000</v>
@@ -1413,10 +841,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C13" s="3">
         <v>2000</v>
@@ -1425,10 +853,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C14" s="3">
         <v>2000</v>
@@ -1437,10 +865,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>5</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C15" s="3">
         <v>2000</v>
@@ -1449,10 +877,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>33</v>
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C16" s="3">
         <v>2000</v>
@@ -1461,10 +889,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>35</v>
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C17" s="3">
         <v>2000</v>
@@ -1473,10 +901,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C18" s="3">
         <v>2000</v>
@@ -1485,10 +913,10 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>39</v>
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C19" s="3">
         <v>2000</v>
@@ -1497,10 +925,10 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>41</v>
+        <v>6</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C20" s="3">
         <v>2000</v>
@@ -1509,10 +937,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>43</v>
+        <v>6</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C21" s="3">
         <v>2000</v>
@@ -1521,10 +949,10 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>6</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="C22" s="3">
         <v>2000</v>
@@ -1533,10 +961,10 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>47</v>
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>87</v>
       </c>
       <c r="C23" s="3">
         <v>2000</v>
@@ -1545,10 +973,10 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>49</v>
+        <v>6</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C24" s="3">
         <v>2000</v>
@@ -1557,10 +985,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>51</v>
+        <v>6</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C25" s="3">
         <v>2000</v>
@@ -1569,10 +997,10 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>53</v>
+        <v>6</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C26" s="3">
         <v>2000</v>
@@ -1581,10 +1009,10 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C27" s="3">
         <v>2000</v>
@@ -1593,10 +1021,10 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>57</v>
+        <v>6</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C28" s="3">
         <v>2000</v>
@@ -1605,10 +1033,10 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>59</v>
+        <v>6</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C29" s="3">
         <v>2000</v>
@@ -1617,10 +1045,10 @@
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>61</v>
+        <v>7</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C30" s="3">
         <v>2000</v>
@@ -1629,10 +1057,10 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>63</v>
+        <v>7</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C31" s="3">
         <v>2000</v>
@@ -1641,10 +1069,10 @@
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>65</v>
+        <v>7</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C32" s="3">
         <v>2000</v>
@@ -1653,10 +1081,10 @@
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>67</v>
+        <v>7</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C33" s="3">
         <v>2000</v>
@@ -1665,10 +1093,10 @@
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B34" s="4" t="s">
-        <v>69</v>
+        <v>7</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C34" s="3">
         <v>2000</v>
@@ -1677,10 +1105,10 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>71</v>
+        <v>7</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C35" s="3">
         <v>2000</v>
@@ -1689,10 +1117,10 @@
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>73</v>
+        <v>7</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C36" s="3">
         <v>2000</v>
@@ -1701,10 +1129,10 @@
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>75</v>
+        <v>7</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C37" s="3">
         <v>2000</v>
@@ -1713,10 +1141,10 @@
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>77</v>
+        <v>7</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C38" s="3">
         <v>2000</v>
@@ -1725,10 +1153,10 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>79</v>
+        <v>7</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C39" s="3">
         <v>2000</v>
@@ -1737,10 +1165,10 @@
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>81</v>
+        <v>8</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C40" s="3">
         <v>2000</v>
@@ -1749,10 +1177,10 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>83</v>
+        <v>8</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C41" s="3">
         <v>2000</v>
@@ -1761,10 +1189,10 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>85</v>
+        <v>8</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C42" s="3">
         <v>2000</v>
@@ -1773,9 +1201,9 @@
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B43" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>87</v>
       </c>
       <c r="C43" s="3">
@@ -1785,10 +1213,10 @@
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>89</v>
+        <v>8</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C44" s="3">
         <v>2000</v>
@@ -1797,10 +1225,10 @@
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>91</v>
+        <v>8</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>87</v>
       </c>
       <c r="C45" s="3">
         <v>2000</v>
@@ -1809,10 +1237,10 @@
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>93</v>
+        <v>8</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
       </c>
       <c r="C46" s="3">
         <v>2000</v>
@@ -1821,10 +1249,10 @@
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>95</v>
+        <v>8</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C47" s="3">
         <v>2000</v>
@@ -1833,10 +1261,10 @@
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>97</v>
+        <v>9</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C48" s="3">
         <v>2000</v>
@@ -1845,10 +1273,10 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B49" s="4" t="s">
-        <v>99</v>
+        <v>9</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C49" s="3">
         <v>2000</v>
@@ -1857,10 +1285,10 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>101</v>
+        <v>9</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C50" s="3">
         <v>2000</v>
@@ -1869,10 +1297,10 @@
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>103</v>
+        <v>9</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C51" s="3">
         <v>2000</v>
@@ -1881,10 +1309,10 @@
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>105</v>
+        <v>9</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C52" s="3">
         <v>2000</v>
@@ -1893,10 +1321,10 @@
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>107</v>
+        <v>9</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C53" s="3">
         <v>2000</v>
@@ -1905,10 +1333,10 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>109</v>
+        <v>9</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C54" s="3">
         <v>2000</v>
@@ -1917,10 +1345,10 @@
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>111</v>
+        <v>9</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C55" s="3">
         <v>2000</v>
@@ -1929,10 +1357,10 @@
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>113</v>
+        <v>9</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C56" s="3">
         <v>2000</v>
@@ -1941,10 +1369,10 @@
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>115</v>
+        <v>9</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C57" s="3">
         <v>2000</v>
@@ -1953,10 +1381,10 @@
     </row>
     <row r="58" spans="1:4">
       <c r="A58" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>117</v>
+        <v>9</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>88</v>
       </c>
       <c r="C58" s="3">
         <v>2000</v>
@@ -1965,10 +1393,10 @@
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>119</v>
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>5198483851037</v>
       </c>
       <c r="C59" s="3">
         <v>2000</v>
@@ -1977,10 +1405,10 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>121</v>
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>5198483851037</v>
       </c>
       <c r="C60" s="3">
         <v>2000</v>
@@ -1989,10 +1417,10 @@
     </row>
     <row r="61" spans="1:4">
       <c r="A61" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>123</v>
+        <v>10</v>
+      </c>
+      <c r="B61" s="5">
+        <v>5198483851037</v>
       </c>
       <c r="C61" s="3">
         <v>2000</v>
@@ -2001,10 +1429,10 @@
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>125</v>
+        <v>10</v>
+      </c>
+      <c r="B62" s="5">
+        <v>5198483851037</v>
       </c>
       <c r="C62" s="3">
         <v>2000</v>
@@ -2013,10 +1441,10 @@
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>127</v>
+        <v>10</v>
+      </c>
+      <c r="B63" s="5">
+        <v>5198483851037</v>
       </c>
       <c r="C63" s="3">
         <v>2000</v>
@@ -2025,10 +1453,10 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>129</v>
+        <v>10</v>
+      </c>
+      <c r="B64" s="5">
+        <v>5198483851037</v>
       </c>
       <c r="C64" s="3">
         <v>2000</v>
@@ -2037,10 +1465,10 @@
     </row>
     <row r="65" spans="1:4">
       <c r="A65" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="B65" s="4" t="s">
-        <v>131</v>
+        <v>10</v>
+      </c>
+      <c r="B65" s="5">
+        <v>5198483851037</v>
       </c>
       <c r="C65" s="3">
         <v>2000</v>
@@ -2049,10 +1477,10 @@
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="B66" s="4" t="s">
-        <v>133</v>
+        <v>10</v>
+      </c>
+      <c r="B66" s="5">
+        <v>5198483851037</v>
       </c>
       <c r="C66" s="3">
         <v>2000</v>
@@ -2061,10 +1489,10 @@
     </row>
     <row r="67" spans="1:4">
       <c r="A67" s="3" t="s">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>135</v>
+        <v>11</v>
       </c>
       <c r="C67" s="3">
         <v>2000</v>
@@ -2073,10 +1501,10 @@
     </row>
     <row r="68" spans="1:4">
       <c r="A68" s="3" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>137</v>
+        <v>12</v>
       </c>
       <c r="C68" s="3">
         <v>2000</v>
@@ -2085,10 +1513,10 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69" s="3" t="s">
-        <v>138</v>
+        <v>10</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>139</v>
+        <v>13</v>
       </c>
       <c r="C69" s="3">
         <v>2000</v>
@@ -2097,10 +1525,10 @@
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
-        <v>140</v>
+        <v>10</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>141</v>
+        <v>14</v>
       </c>
       <c r="C70" s="3">
         <v>2000</v>
@@ -2109,10 +1537,10 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
-        <v>142</v>
+        <v>10</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>143</v>
+        <v>15</v>
       </c>
       <c r="C71" s="3">
         <v>2000</v>
@@ -2121,10 +1549,10 @@
     </row>
     <row r="72" spans="1:4">
       <c r="A72" s="3" t="s">
-        <v>144</v>
+        <v>10</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>145</v>
+        <v>16</v>
       </c>
       <c r="C72" s="3">
         <v>2000</v>
@@ -2133,10 +1561,10 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73" s="3" t="s">
-        <v>146</v>
+        <v>10</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>147</v>
+        <v>17</v>
       </c>
       <c r="C73" s="3">
         <v>2000</v>
@@ -2145,10 +1573,10 @@
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
-        <v>148</v>
+        <v>10</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>149</v>
+        <v>18</v>
       </c>
       <c r="C74" s="3">
         <v>2000</v>
@@ -2157,10 +1585,10 @@
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>151</v>
+        <v>19</v>
       </c>
       <c r="C75" s="3">
         <v>2000</v>
@@ -2169,10 +1597,10 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="3" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>153</v>
+        <v>20</v>
       </c>
       <c r="C76" s="3">
         <v>2000</v>
@@ -2181,10 +1609,10 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77" s="3" t="s">
-        <v>154</v>
+        <v>10</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>155</v>
+        <v>21</v>
       </c>
       <c r="C77" s="3">
         <v>2000</v>
@@ -2193,10 +1621,10 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78" s="3" t="s">
-        <v>156</v>
+        <v>10</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>157</v>
+        <v>22</v>
       </c>
       <c r="C78" s="3">
         <v>2000</v>
@@ -2205,10 +1633,10 @@
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="3" t="s">
-        <v>158</v>
+        <v>10</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>159</v>
+        <v>23</v>
       </c>
       <c r="C79" s="3">
         <v>2000</v>
@@ -2217,10 +1645,10 @@
     </row>
     <row r="80" spans="1:4">
       <c r="A80" s="3" t="s">
-        <v>160</v>
+        <v>10</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>161</v>
+        <v>24</v>
       </c>
       <c r="C80" s="3">
         <v>2000</v>
@@ -2229,10 +1657,10 @@
     </row>
     <row r="81" spans="1:4">
       <c r="A81" s="3" t="s">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>163</v>
+        <v>25</v>
       </c>
       <c r="C81" s="3">
         <v>2000</v>
@@ -2241,10 +1669,10 @@
     </row>
     <row r="82" spans="1:4">
       <c r="A82" s="3" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>165</v>
+        <v>26</v>
       </c>
       <c r="C82" s="3">
         <v>2000</v>
@@ -2253,10 +1681,10 @@
     </row>
     <row r="83" spans="1:4">
       <c r="A83" s="3" t="s">
-        <v>166</v>
+        <v>10</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>167</v>
+        <v>27</v>
       </c>
       <c r="C83" s="3">
         <v>2000</v>
@@ -2265,10 +1693,10 @@
     </row>
     <row r="84" spans="1:4">
       <c r="A84" s="3" t="s">
-        <v>168</v>
+        <v>10</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>169</v>
+        <v>28</v>
       </c>
       <c r="C84" s="3">
         <v>2000</v>
@@ -2277,10 +1705,10 @@
     </row>
     <row r="85" spans="1:4">
       <c r="A85" s="3" t="s">
-        <v>170</v>
+        <v>10</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>171</v>
+        <v>29</v>
       </c>
       <c r="C85" s="3">
         <v>2000</v>
@@ -2289,10 +1717,10 @@
     </row>
     <row r="86" spans="1:4">
       <c r="A86" s="3" t="s">
-        <v>172</v>
+        <v>10</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>173</v>
+        <v>30</v>
       </c>
       <c r="C86" s="3">
         <v>2000</v>
@@ -2301,10 +1729,10 @@
     </row>
     <row r="87" spans="1:4">
       <c r="A87" s="3" t="s">
-        <v>174</v>
+        <v>10</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>175</v>
+        <v>31</v>
       </c>
       <c r="C87" s="3">
         <v>2000</v>
@@ -2313,10 +1741,10 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88" s="3" t="s">
-        <v>176</v>
+        <v>10</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>177</v>
+        <v>32</v>
       </c>
       <c r="C88" s="3">
         <v>2000</v>
@@ -2325,10 +1753,10 @@
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="3" t="s">
-        <v>178</v>
+        <v>10</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>179</v>
+        <v>33</v>
       </c>
       <c r="C89" s="3">
         <v>2000</v>
@@ -2337,10 +1765,10 @@
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="3" t="s">
-        <v>180</v>
+        <v>10</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>181</v>
+        <v>34</v>
       </c>
       <c r="C90" s="3">
         <v>2000</v>
@@ -2349,10 +1777,10 @@
     </row>
     <row r="91" spans="1:4">
       <c r="A91" s="3" t="s">
-        <v>182</v>
+        <v>10</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>183</v>
+        <v>35</v>
       </c>
       <c r="C91" s="3">
         <v>2000</v>
@@ -2361,10 +1789,10 @@
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="3" t="s">
-        <v>184</v>
+        <v>10</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>185</v>
+        <v>36</v>
       </c>
       <c r="C92" s="3">
         <v>2000</v>
@@ -2373,10 +1801,10 @@
     </row>
     <row r="93" spans="1:4">
       <c r="A93" s="3" t="s">
-        <v>186</v>
+        <v>10</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>187</v>
+        <v>37</v>
       </c>
       <c r="C93" s="3">
         <v>2000</v>
@@ -2385,10 +1813,10 @@
     </row>
     <row r="94" spans="1:4">
       <c r="A94" s="3" t="s">
-        <v>188</v>
+        <v>10</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>189</v>
+        <v>38</v>
       </c>
       <c r="C94" s="3">
         <v>2000</v>
@@ -2397,10 +1825,10 @@
     </row>
     <row r="95" spans="1:4">
       <c r="A95" s="3" t="s">
-        <v>190</v>
+        <v>10</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>191</v>
+        <v>39</v>
       </c>
       <c r="C95" s="3">
         <v>2000</v>
@@ -2409,10 +1837,10 @@
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="3" t="s">
-        <v>192</v>
+        <v>10</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>193</v>
+        <v>40</v>
       </c>
       <c r="C96" s="3">
         <v>2000</v>
@@ -2421,10 +1849,10 @@
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="3" t="s">
-        <v>194</v>
+        <v>10</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>195</v>
+        <v>41</v>
       </c>
       <c r="C97" s="3">
         <v>2000</v>
@@ -2433,10 +1861,10 @@
     </row>
     <row r="98" spans="1:4">
       <c r="A98" s="3" t="s">
-        <v>196</v>
+        <v>10</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>197</v>
+        <v>42</v>
       </c>
       <c r="C98" s="3">
         <v>2000</v>
@@ -2445,10 +1873,10 @@
     </row>
     <row r="99" spans="1:4">
       <c r="A99" s="3" t="s">
-        <v>198</v>
+        <v>10</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>199</v>
+        <v>43</v>
       </c>
       <c r="C99" s="3">
         <v>2000</v>
@@ -2457,10 +1885,10 @@
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="3" t="s">
-        <v>200</v>
+        <v>10</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>201</v>
+        <v>44</v>
       </c>
       <c r="C100" s="3">
         <v>2000</v>
@@ -2469,10 +1897,10 @@
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="3" t="s">
-        <v>202</v>
+        <v>10</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>203</v>
+        <v>45</v>
       </c>
       <c r="C101" s="3">
         <v>2000</v>
@@ -2481,10 +1909,10 @@
     </row>
     <row r="102" spans="1:4">
       <c r="A102" s="3" t="s">
-        <v>204</v>
+        <v>10</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>205</v>
+        <v>46</v>
       </c>
       <c r="C102" s="3">
         <v>2000</v>
@@ -2493,10 +1921,10 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="3" t="s">
-        <v>206</v>
+        <v>10</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>207</v>
+        <v>47</v>
       </c>
       <c r="C103" s="3">
         <v>2000</v>
@@ -2505,10 +1933,10 @@
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="3" t="s">
-        <v>208</v>
+        <v>10</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>209</v>
+        <v>48</v>
       </c>
       <c r="C104" s="3">
         <v>2000</v>
@@ -2517,10 +1945,10 @@
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="3" t="s">
-        <v>210</v>
+        <v>10</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>211</v>
+        <v>49</v>
       </c>
       <c r="C105" s="3">
         <v>2000</v>
@@ -2529,10 +1957,10 @@
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="3" t="s">
-        <v>212</v>
+        <v>10</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>213</v>
+        <v>50</v>
       </c>
       <c r="C106" s="3">
         <v>2000</v>
@@ -2541,10 +1969,10 @@
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="3" t="s">
-        <v>214</v>
+        <v>10</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>215</v>
+        <v>51</v>
       </c>
       <c r="C107" s="3">
         <v>2000</v>
@@ -2553,10 +1981,10 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="3" t="s">
-        <v>216</v>
+        <v>10</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>217</v>
+        <v>52</v>
       </c>
       <c r="C108" s="3">
         <v>2000</v>
@@ -2565,10 +1993,10 @@
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="3" t="s">
-        <v>218</v>
+        <v>10</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>219</v>
+        <v>53</v>
       </c>
       <c r="C109" s="3">
         <v>2000</v>
@@ -2577,10 +2005,10 @@
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="3" t="s">
-        <v>220</v>
+        <v>10</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>221</v>
+        <v>54</v>
       </c>
       <c r="C110" s="3">
         <v>2000</v>
@@ -2589,10 +2017,10 @@
     </row>
     <row r="111" spans="1:4">
       <c r="A111" s="3" t="s">
-        <v>222</v>
+        <v>55</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>223</v>
+        <v>56</v>
       </c>
       <c r="C111" s="3">
         <v>2000</v>
@@ -2601,10 +2029,10 @@
     </row>
     <row r="112" spans="1:4">
       <c r="A112" s="3" t="s">
-        <v>224</v>
+        <v>55</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>225</v>
+        <v>57</v>
       </c>
       <c r="C112" s="3">
         <v>2000</v>
@@ -2613,10 +2041,10 @@
     </row>
     <row r="113" spans="1:4">
       <c r="A113" s="3" t="s">
-        <v>226</v>
+        <v>55</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>227</v>
+        <v>58</v>
       </c>
       <c r="C113" s="3">
         <v>2000</v>
@@ -2625,10 +2053,10 @@
     </row>
     <row r="114" spans="1:4">
       <c r="A114" s="3" t="s">
-        <v>228</v>
+        <v>55</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>229</v>
+        <v>59</v>
       </c>
       <c r="C114" s="3">
         <v>2000</v>
@@ -2637,10 +2065,10 @@
     </row>
     <row r="115" spans="1:4">
       <c r="A115" s="3" t="s">
-        <v>230</v>
+        <v>55</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>231</v>
+        <v>60</v>
       </c>
       <c r="C115" s="3">
         <v>2000</v>
@@ -2649,10 +2077,10 @@
     </row>
     <row r="116" spans="1:4">
       <c r="A116" s="3" t="s">
-        <v>232</v>
+        <v>55</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>233</v>
+        <v>61</v>
       </c>
       <c r="C116" s="3">
         <v>2000</v>
@@ -2661,10 +2089,10 @@
     </row>
     <row r="117" spans="1:4">
       <c r="A117" s="3" t="s">
-        <v>234</v>
+        <v>55</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>235</v>
+        <v>62</v>
       </c>
       <c r="C117" s="3">
         <v>2000</v>
@@ -2673,10 +2101,10 @@
     </row>
     <row r="118" spans="1:4">
       <c r="A118" s="3" t="s">
-        <v>236</v>
+        <v>55</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>237</v>
+        <v>63</v>
       </c>
       <c r="C118" s="3">
         <v>2000</v>
@@ -2685,10 +2113,10 @@
     </row>
     <row r="119" spans="1:4">
       <c r="A119" s="3" t="s">
-        <v>238</v>
+        <v>55</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>239</v>
+        <v>64</v>
       </c>
       <c r="C119" s="3">
         <v>2000</v>
@@ -2697,10 +2125,10 @@
     </row>
     <row r="120" spans="1:4">
       <c r="A120" s="3" t="s">
-        <v>240</v>
+        <v>55</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>241</v>
+        <v>65</v>
       </c>
       <c r="C120" s="3">
         <v>2000</v>
@@ -2709,10 +2137,10 @@
     </row>
     <row r="121" spans="1:4">
       <c r="A121" s="3" t="s">
-        <v>242</v>
+        <v>55</v>
       </c>
       <c r="B121" s="4" t="s">
-        <v>243</v>
+        <v>66</v>
       </c>
       <c r="C121" s="3">
         <v>2000</v>
@@ -2721,10 +2149,10 @@
     </row>
     <row r="122" spans="1:4">
       <c r="A122" s="3" t="s">
-        <v>244</v>
+        <v>55</v>
       </c>
       <c r="B122" s="4" t="s">
-        <v>245</v>
+        <v>67</v>
       </c>
       <c r="C122" s="3">
         <v>2000</v>
@@ -2733,10 +2161,10 @@
     </row>
     <row r="123" spans="1:4">
       <c r="A123" s="3" t="s">
-        <v>246</v>
+        <v>55</v>
       </c>
       <c r="B123" s="4" t="s">
-        <v>247</v>
+        <v>68</v>
       </c>
       <c r="C123" s="3">
         <v>2000</v>
@@ -2745,10 +2173,10 @@
     </row>
     <row r="124" spans="1:4">
       <c r="A124" s="3" t="s">
-        <v>248</v>
+        <v>55</v>
       </c>
       <c r="B124" s="4" t="s">
-        <v>249</v>
+        <v>69</v>
       </c>
       <c r="C124" s="3">
         <v>2000</v>
@@ -2757,10 +2185,10 @@
     </row>
     <row r="125" spans="1:4">
       <c r="A125" s="3" t="s">
-        <v>250</v>
+        <v>55</v>
       </c>
       <c r="B125" s="4" t="s">
-        <v>251</v>
+        <v>70</v>
       </c>
       <c r="C125" s="3">
         <v>2000</v>
@@ -2769,10 +2197,10 @@
     </row>
     <row r="126" spans="1:4">
       <c r="A126" s="3" t="s">
-        <v>252</v>
+        <v>55</v>
       </c>
       <c r="B126" s="4" t="s">
-        <v>253</v>
+        <v>71</v>
       </c>
       <c r="C126" s="3">
         <v>2000</v>
@@ -2781,10 +2209,10 @@
     </row>
     <row r="127" spans="1:4">
       <c r="A127" s="3" t="s">
-        <v>254</v>
+        <v>55</v>
       </c>
       <c r="B127" s="4" t="s">
-        <v>255</v>
+        <v>72</v>
       </c>
       <c r="C127" s="3">
         <v>2000</v>
@@ -2793,10 +2221,10 @@
     </row>
     <row r="128" spans="1:4">
       <c r="A128" s="3" t="s">
-        <v>256</v>
+        <v>55</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>257</v>
+        <v>73</v>
       </c>
       <c r="C128" s="3">
         <v>2000</v>
@@ -2805,10 +2233,10 @@
     </row>
     <row r="129" spans="1:4">
       <c r="A129" s="3" t="s">
-        <v>258</v>
+        <v>55</v>
       </c>
       <c r="B129" s="4" t="s">
-        <v>259</v>
+        <v>74</v>
       </c>
       <c r="C129" s="3">
         <v>2000</v>
@@ -2817,10 +2245,10 @@
     </row>
     <row r="130" spans="1:4">
       <c r="A130" s="3" t="s">
-        <v>260</v>
+        <v>55</v>
       </c>
       <c r="B130" s="4" t="s">
-        <v>261</v>
+        <v>75</v>
       </c>
       <c r="C130" s="3">
         <v>2000</v>
@@ -2829,10 +2257,10 @@
     </row>
     <row r="131" spans="1:4">
       <c r="A131" s="3" t="s">
-        <v>262</v>
+        <v>55</v>
       </c>
       <c r="B131" s="4" t="s">
-        <v>263</v>
+        <v>76</v>
       </c>
       <c r="C131" s="3">
         <v>2000</v>
@@ -2841,10 +2269,10 @@
     </row>
     <row r="132" spans="1:4">
       <c r="A132" s="3" t="s">
-        <v>264</v>
+        <v>55</v>
       </c>
       <c r="B132" s="4" t="s">
-        <v>265</v>
+        <v>77</v>
       </c>
       <c r="C132" s="3">
         <v>2000</v>
@@ -2853,10 +2281,10 @@
     </row>
     <row r="133" spans="1:4">
       <c r="A133" s="3" t="s">
-        <v>266</v>
+        <v>55</v>
       </c>
       <c r="B133" s="4" t="s">
-        <v>267</v>
+        <v>78</v>
       </c>
       <c r="C133" s="3">
         <v>2000</v>
@@ -2865,10 +2293,10 @@
     </row>
     <row r="134" spans="1:4">
       <c r="A134" s="3" t="s">
-        <v>268</v>
+        <v>55</v>
       </c>
       <c r="B134" s="4" t="s">
-        <v>269</v>
+        <v>79</v>
       </c>
       <c r="C134" s="3">
         <v>2000</v>
@@ -2877,10 +2305,10 @@
     </row>
     <row r="135" spans="1:4">
       <c r="A135" s="3" t="s">
-        <v>270</v>
+        <v>55</v>
       </c>
       <c r="B135" s="4" t="s">
-        <v>271</v>
+        <v>80</v>
       </c>
       <c r="C135" s="3">
         <v>2000</v>
@@ -2889,10 +2317,10 @@
     </row>
     <row r="136" spans="1:4">
       <c r="A136" s="3" t="s">
-        <v>272</v>
+        <v>55</v>
       </c>
       <c r="B136" s="4" t="s">
-        <v>273</v>
+        <v>81</v>
       </c>
       <c r="C136" s="3">
         <v>2000</v>
@@ -2901,10 +2329,10 @@
     </row>
     <row r="137" spans="1:4">
       <c r="A137" s="3" t="s">
-        <v>274</v>
+        <v>55</v>
       </c>
       <c r="B137" s="4" t="s">
-        <v>275</v>
+        <v>82</v>
       </c>
       <c r="C137" s="3">
         <v>2000</v>
@@ -2913,10 +2341,10 @@
     </row>
     <row r="138" spans="1:4">
       <c r="A138" s="3" t="s">
-        <v>276</v>
+        <v>55</v>
       </c>
       <c r="B138" s="4" t="s">
-        <v>277</v>
+        <v>83</v>
       </c>
       <c r="C138" s="3">
         <v>2000</v>
@@ -2925,10 +2353,10 @@
     </row>
     <row r="139" spans="1:4">
       <c r="A139" s="3" t="s">
-        <v>278</v>
+        <v>55</v>
       </c>
       <c r="B139" s="4" t="s">
-        <v>279</v>
+        <v>84</v>
       </c>
       <c r="C139" s="3">
         <v>2000</v>
@@ -2937,10 +2365,10 @@
     </row>
     <row r="140" spans="1:4">
       <c r="A140" s="3" t="s">
-        <v>280</v>
+        <v>55</v>
       </c>
       <c r="B140" s="4" t="s">
-        <v>281</v>
+        <v>85</v>
       </c>
       <c r="C140" s="3">
         <v>2000</v>
@@ -2949,6 +2377,7 @@
     </row>
   </sheetData>
   <sheetProtection sheet="1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>